<commit_message>
fix: deidentify personal emails
</commit_message>
<xml_diff>
--- a/testing/cypress/fixtures/Test Data.xlsx
+++ b/testing/cypress/fixtures/Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\sso-requests-e2e\testing\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF229244-BDDC-4A61-8ADF-0B25BBA41369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D2C22C-249C-4CC0-9B56-F6307B8C967E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -756,27 +756,6 @@
     <t>Team 1</t>
   </si>
   <si>
-    <t>roland.stens@gov.bc.ca</t>
-  </si>
-  <si>
-    <t>roland.stens@gmail.com</t>
-  </si>
-  <si>
-    <t>roland.stens+test1@gmail.com</t>
-  </si>
-  <si>
-    <t>roland.stens+test2@gmail.com</t>
-  </si>
-  <si>
-    <t>roland.stens+test3@gmail.com</t>
-  </si>
-  <si>
-    <t>roland.stens+test4@gmail.com</t>
-  </si>
-  <si>
-    <t>roland.stens+test5@gmail.com</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
@@ -789,15 +768,9 @@
     <t>Team 1 Updated</t>
   </si>
   <si>
-    <t>roland.stens+test6@gmail.com</t>
-  </si>
-  <si>
     <t>Admin</t>
   </si>
   <si>
-    <t>roland.stens+test7@gmail.com</t>
-  </si>
-  <si>
     <t>Member</t>
   </si>
   <si>
@@ -928,6 +901,33 @@
   </si>
   <si>
     <t>update.deleteuser.0.useremail.0</t>
+  </si>
+  <si>
+    <t>test.user@gov.bc.ca</t>
+  </si>
+  <si>
+    <t>test.user@gmail.com</t>
+  </si>
+  <si>
+    <t>test.user+test1@gmail.com</t>
+  </si>
+  <si>
+    <t>test.user+test2@gmail.com</t>
+  </si>
+  <si>
+    <t>test.user+test3@gmail.com</t>
+  </si>
+  <si>
+    <t>test.user+test4@gmail.com</t>
+  </si>
+  <si>
+    <t>test.user+test5@gmail.com</t>
+  </si>
+  <si>
+    <t>test.user+test6@gmail.com</t>
+  </si>
+  <si>
+    <t>test.user+test7@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -5819,7 +5819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F407C59-92A7-47A4-923E-B6082F6C20A1}">
   <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
@@ -5851,46 +5851,46 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>29</v>
@@ -5902,19 +5902,19 @@
         <v>33</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>52</v>
@@ -5931,70 +5931,70 @@
         <v>240</v>
       </c>
       <c r="C2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E2" t="s">
+        <v>292</v>
+      </c>
+      <c r="F2" t="s">
+        <v>293</v>
+      </c>
+      <c r="G2" t="s">
+        <v>294</v>
+      </c>
+      <c r="H2" t="s">
+        <v>295</v>
+      </c>
+      <c r="I2" t="s">
+        <v>296</v>
+      </c>
+      <c r="J2" t="s">
         <v>241</v>
       </c>
-      <c r="D2" t="s">
+      <c r="K2" t="s">
+        <v>241</v>
+      </c>
+      <c r="L2" t="s">
         <v>242</v>
       </c>
-      <c r="E2" t="s">
+      <c r="M2" t="s">
+        <v>242</v>
+      </c>
+      <c r="N2" t="s">
+        <v>242</v>
+      </c>
+      <c r="O2" t="s">
+        <v>242</v>
+      </c>
+      <c r="P2" t="s">
+        <v>242</v>
+      </c>
+      <c r="R2" t="s">
         <v>243</v>
       </c>
-      <c r="F2" t="s">
+      <c r="S2" t="s">
         <v>244</v>
       </c>
-      <c r="G2" t="s">
+      <c r="T2" t="s">
+        <v>297</v>
+      </c>
+      <c r="U2" t="s">
         <v>245</v>
       </c>
-      <c r="H2" t="s">
+      <c r="V2" t="s">
+        <v>298</v>
+      </c>
+      <c r="W2" t="s">
         <v>246</v>
       </c>
-      <c r="I2" t="s">
-        <v>247</v>
-      </c>
-      <c r="J2" t="s">
-        <v>248</v>
-      </c>
-      <c r="K2" t="s">
-        <v>248</v>
-      </c>
-      <c r="L2" t="s">
-        <v>249</v>
-      </c>
-      <c r="M2" t="s">
-        <v>249</v>
-      </c>
-      <c r="N2" t="s">
-        <v>249</v>
-      </c>
-      <c r="O2" t="s">
-        <v>249</v>
-      </c>
-      <c r="P2" t="s">
-        <v>249</v>
-      </c>
-      <c r="R2" t="s">
-        <v>250</v>
-      </c>
-      <c r="S2" t="s">
-        <v>251</v>
-      </c>
-      <c r="T2" t="s">
-        <v>252</v>
-      </c>
-      <c r="U2" t="s">
-        <v>253</v>
-      </c>
-      <c r="V2" t="s">
-        <v>254</v>
-      </c>
-      <c r="W2" t="s">
-        <v>255</v>
-      </c>
       <c r="X2" t="s">
-        <v>242</v>
+        <v>291</v>
       </c>
       <c r="Y2" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="Z2" t="b">
         <v>1</v>
@@ -6002,46 +6002,46 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="B3" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="C3" t="s">
+        <v>290</v>
+      </c>
+      <c r="D3" t="s">
+        <v>291</v>
+      </c>
+      <c r="J3" t="s">
         <v>241</v>
       </c>
-      <c r="D3" t="s">
-        <v>242</v>
-      </c>
-      <c r="J3" t="s">
-        <v>248</v>
-      </c>
       <c r="K3" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="R3" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="S3" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="T3" t="s">
-        <v>252</v>
+        <v>297</v>
       </c>
       <c r="U3" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="V3" t="s">
-        <v>254</v>
+        <v>298</v>
       </c>
       <c r="W3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="X3" t="s">
-        <v>242</v>
+        <v>291</v>
       </c>
       <c r="Y3" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="Z3" t="b">
         <v>1</v>
@@ -6049,52 +6049,52 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B4" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="C4" t="s">
+        <v>290</v>
+      </c>
+      <c r="D4" t="s">
+        <v>291</v>
+      </c>
+      <c r="E4" t="s">
+        <v>292</v>
+      </c>
+      <c r="J4" t="s">
         <v>241</v>
       </c>
-      <c r="D4" t="s">
+      <c r="K4" t="s">
         <v>242</v>
       </c>
-      <c r="E4" t="s">
-        <v>243</v>
-      </c>
-      <c r="J4" t="s">
-        <v>248</v>
-      </c>
-      <c r="K4" t="s">
-        <v>249</v>
-      </c>
       <c r="L4" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="R4" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="S4" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="T4" t="s">
-        <v>252</v>
+        <v>297</v>
       </c>
       <c r="U4" t="s">
+        <v>245</v>
+      </c>
+      <c r="V4" t="s">
+        <v>298</v>
+      </c>
+      <c r="W4" t="s">
+        <v>246</v>
+      </c>
+      <c r="X4" t="s">
+        <v>291</v>
+      </c>
+      <c r="Y4" t="s">
         <v>253</v>
-      </c>
-      <c r="V4" t="s">
-        <v>254</v>
-      </c>
-      <c r="W4" t="s">
-        <v>255</v>
-      </c>
-      <c r="X4" t="s">
-        <v>242</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>262</v>
       </c>
       <c r="Z4" t="b">
         <v>1</v>
@@ -6102,58 +6102,58 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="B5" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="C5" t="s">
+        <v>290</v>
+      </c>
+      <c r="D5" t="s">
+        <v>291</v>
+      </c>
+      <c r="E5" t="s">
+        <v>292</v>
+      </c>
+      <c r="F5" t="s">
+        <v>293</v>
+      </c>
+      <c r="J5" t="s">
         <v>241</v>
       </c>
-      <c r="D5" t="s">
+      <c r="K5" t="s">
         <v>242</v>
       </c>
-      <c r="E5" t="s">
-        <v>243</v>
-      </c>
-      <c r="F5" t="s">
-        <v>244</v>
-      </c>
-      <c r="J5" t="s">
-        <v>248</v>
-      </c>
-      <c r="K5" t="s">
-        <v>249</v>
-      </c>
       <c r="L5" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="M5" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="R5" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="S5" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="T5" t="s">
-        <v>252</v>
+        <v>297</v>
       </c>
       <c r="U5" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="V5" t="s">
-        <v>254</v>
+        <v>298</v>
       </c>
       <c r="W5" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="X5" t="s">
-        <v>242</v>
+        <v>291</v>
       </c>
       <c r="Y5" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="Z5" t="b">
         <v>1</v>
@@ -6161,64 +6161,64 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="B6" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="C6" t="s">
+        <v>290</v>
+      </c>
+      <c r="D6" t="s">
+        <v>291</v>
+      </c>
+      <c r="E6" t="s">
+        <v>292</v>
+      </c>
+      <c r="F6" t="s">
+        <v>293</v>
+      </c>
+      <c r="G6" t="s">
+        <v>294</v>
+      </c>
+      <c r="J6" t="s">
         <v>241</v>
       </c>
-      <c r="D6" t="s">
+      <c r="K6" t="s">
         <v>242</v>
       </c>
-      <c r="E6" t="s">
-        <v>243</v>
-      </c>
-      <c r="F6" t="s">
-        <v>244</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="L6" t="s">
+        <v>242</v>
+      </c>
+      <c r="M6" t="s">
+        <v>242</v>
+      </c>
+      <c r="N6" t="s">
+        <v>242</v>
+      </c>
+      <c r="R6" t="s">
+        <v>261</v>
+      </c>
+      <c r="S6" t="s">
+        <v>262</v>
+      </c>
+      <c r="T6" t="s">
+        <v>297</v>
+      </c>
+      <c r="U6" t="s">
         <v>245</v>
       </c>
-      <c r="J6" t="s">
-        <v>248</v>
-      </c>
-      <c r="K6" t="s">
-        <v>249</v>
-      </c>
-      <c r="L6" t="s">
-        <v>249</v>
-      </c>
-      <c r="M6" t="s">
-        <v>249</v>
-      </c>
-      <c r="N6" t="s">
-        <v>249</v>
-      </c>
-      <c r="R6" t="s">
-        <v>270</v>
-      </c>
-      <c r="S6" t="s">
-        <v>271</v>
-      </c>
-      <c r="T6" t="s">
-        <v>252</v>
-      </c>
-      <c r="U6" t="s">
-        <v>253</v>
-      </c>
       <c r="V6" t="s">
-        <v>254</v>
+        <v>298</v>
       </c>
       <c r="W6" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="X6" t="s">
-        <v>242</v>
+        <v>291</v>
       </c>
       <c r="Y6" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="Z6" t="b">
         <v>1</v>
@@ -6226,70 +6226,70 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="B7" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="C7" t="s">
+        <v>290</v>
+      </c>
+      <c r="D7" t="s">
+        <v>291</v>
+      </c>
+      <c r="E7" t="s">
+        <v>292</v>
+      </c>
+      <c r="F7" t="s">
+        <v>293</v>
+      </c>
+      <c r="G7" t="s">
+        <v>294</v>
+      </c>
+      <c r="H7" t="s">
+        <v>295</v>
+      </c>
+      <c r="J7" t="s">
         <v>241</v>
       </c>
-      <c r="D7" t="s">
+      <c r="K7" t="s">
         <v>242</v>
       </c>
-      <c r="E7" t="s">
-        <v>243</v>
-      </c>
-      <c r="F7" t="s">
-        <v>244</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="L7" t="s">
+        <v>242</v>
+      </c>
+      <c r="M7" t="s">
+        <v>242</v>
+      </c>
+      <c r="N7" t="s">
+        <v>242</v>
+      </c>
+      <c r="O7" t="s">
+        <v>242</v>
+      </c>
+      <c r="R7" t="s">
+        <v>265</v>
+      </c>
+      <c r="S7" t="s">
+        <v>266</v>
+      </c>
+      <c r="T7" t="s">
+        <v>297</v>
+      </c>
+      <c r="U7" t="s">
+        <v>246</v>
+      </c>
+      <c r="V7" t="s">
+        <v>298</v>
+      </c>
+      <c r="W7" t="s">
         <v>245</v>
       </c>
-      <c r="H7" t="s">
-        <v>246</v>
-      </c>
-      <c r="J7" t="s">
-        <v>248</v>
-      </c>
-      <c r="K7" t="s">
-        <v>249</v>
-      </c>
-      <c r="L7" t="s">
-        <v>249</v>
-      </c>
-      <c r="M7" t="s">
-        <v>249</v>
-      </c>
-      <c r="N7" t="s">
-        <v>249</v>
-      </c>
-      <c r="O7" t="s">
-        <v>249</v>
-      </c>
-      <c r="R7" t="s">
-        <v>274</v>
-      </c>
-      <c r="S7" t="s">
-        <v>275</v>
-      </c>
-      <c r="T7" t="s">
-        <v>252</v>
-      </c>
-      <c r="U7" t="s">
-        <v>255</v>
-      </c>
-      <c r="V7" t="s">
-        <v>254</v>
-      </c>
-      <c r="W7" t="s">
-        <v>253</v>
-      </c>
       <c r="X7" t="s">
-        <v>242</v>
+        <v>291</v>
       </c>
       <c r="Y7" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="Z7" t="b">
         <v>1</v>
@@ -6297,76 +6297,76 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B8" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="C8" t="s">
+        <v>290</v>
+      </c>
+      <c r="D8" t="s">
+        <v>291</v>
+      </c>
+      <c r="E8" t="s">
+        <v>292</v>
+      </c>
+      <c r="F8" t="s">
+        <v>293</v>
+      </c>
+      <c r="G8" t="s">
+        <v>294</v>
+      </c>
+      <c r="H8" t="s">
+        <v>295</v>
+      </c>
+      <c r="I8" t="s">
+        <v>296</v>
+      </c>
+      <c r="J8" t="s">
         <v>241</v>
       </c>
-      <c r="D8" t="s">
+      <c r="K8" t="s">
+        <v>241</v>
+      </c>
+      <c r="L8" t="s">
         <v>242</v>
       </c>
-      <c r="E8" t="s">
-        <v>243</v>
-      </c>
-      <c r="F8" t="s">
-        <v>244</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="M8" t="s">
+        <v>242</v>
+      </c>
+      <c r="N8" t="s">
+        <v>242</v>
+      </c>
+      <c r="O8" t="s">
+        <v>242</v>
+      </c>
+      <c r="P8" t="s">
+        <v>242</v>
+      </c>
+      <c r="R8" t="s">
+        <v>269</v>
+      </c>
+      <c r="S8" t="s">
+        <v>270</v>
+      </c>
+      <c r="T8" t="s">
+        <v>297</v>
+      </c>
+      <c r="U8" t="s">
         <v>245</v>
       </c>
-      <c r="H8" t="s">
+      <c r="V8" t="s">
+        <v>298</v>
+      </c>
+      <c r="W8" t="s">
         <v>246</v>
       </c>
-      <c r="I8" t="s">
-        <v>247</v>
-      </c>
-      <c r="J8" t="s">
-        <v>248</v>
-      </c>
-      <c r="K8" t="s">
-        <v>248</v>
-      </c>
-      <c r="L8" t="s">
-        <v>249</v>
-      </c>
-      <c r="M8" t="s">
-        <v>249</v>
-      </c>
-      <c r="N8" t="s">
-        <v>249</v>
-      </c>
-      <c r="O8" t="s">
-        <v>249</v>
-      </c>
-      <c r="P8" t="s">
-        <v>249</v>
-      </c>
-      <c r="R8" t="s">
-        <v>278</v>
-      </c>
-      <c r="S8" t="s">
-        <v>279</v>
-      </c>
-      <c r="T8" t="s">
-        <v>252</v>
-      </c>
-      <c r="U8" t="s">
-        <v>253</v>
-      </c>
-      <c r="V8" t="s">
-        <v>254</v>
-      </c>
-      <c r="W8" t="s">
-        <v>255</v>
-      </c>
       <c r="X8" t="s">
-        <v>242</v>
+        <v>291</v>
       </c>
       <c r="Y8" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="Z8" t="b">
         <v>1</v>

</xml_diff>